<commit_message>
Borrar filas innecesarias del Excel
Con un nuevo método en la DAL de Excel se borran las filas innecesarias
de la hoja de cheques y transferencias
</commit_message>
<xml_diff>
--- a/CorteDeSucursales/Plantillas/Plantilla.xlsx
+++ b/CorteDeSucursales/Plantillas/Plantilla.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>SUCURSAL</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>BORRAR</t>
   </si>
 </sst>
 </file>
@@ -589,6 +592,44 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -596,53 +637,15 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,12 +1212,12 @@
       <c r="C22" s="18"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="46"/>
-      <c r="B23" s="46"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="60"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1231,7 +1234,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1243,78 +1246,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:5" ht="6" customHeight="1"/>
     <row r="3" spans="1:5">
       <c r="A3" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="50" t="str">
+      <c r="B3" s="64" t="str">
         <f>Resumen!B1</f>
         <v>Sucursal</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="50" t="str">
+      <c r="B4" s="64" t="str">
         <f>Resumen!B3</f>
         <v>Fecha</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
     </row>
     <row r="5" spans="1:5" ht="6" customHeight="1"/>
     <row r="6" spans="1:5" ht="18">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="49"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="43"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="57" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="54"/>
+      <c r="A8" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="55"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="58"/>
+      <c r="A9" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="64"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63" t="s">
+      <c r="A10" s="59"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="53">
         <f>SUM(D8:D9)</f>
         <v>0</v>
       </c>
@@ -1326,38 +1333,42 @@
       <c r="B12" s="45"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="57" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
+      <c r="A14" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="55"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
+      <c r="A15" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="64"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63" t="s">
+      <c r="A16" s="59"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="53">
         <f>SUM(D14:D15)</f>
         <v>0</v>
       </c>

</xml_diff>